<commit_message>
Added Old Slides + Updated Syllabus
</commit_message>
<xml_diff>
--- a/1_Sylabus/date_helper.xlsx
+++ b/1_Sylabus/date_helper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Teaching\class_intro_to_polsci\1_Sylabus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158A933C-4CF7-4458-8628-0E61EFFF3482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869B7EE7-2B21-45EA-AB49-46A316AA18FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{BB3550EC-397D-4C1A-A975-D7D2733D7A73}"/>
+    <workbookView xWindow="9600" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{BB3550EC-397D-4C1A-A975-D7D2733D7A73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Paste To Document</t>
   </si>
   <si>
-    <t>Quantitative Methoden IV – Anwendung 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">(Präsenz) -Vorstellung und Einführung </t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t xml:space="preserve">(Präsenz) Konzepte und Operationalisierungen </t>
   </si>
   <si>
-    <t xml:space="preserve">(Asynchron+Online) Wahlen und Wähler in Deutschland und der Welt </t>
-  </si>
-  <si>
     <t>(Präsenz) Wer wählt populistische Parteien? + Wissenschaftliches Lesen I</t>
   </si>
   <si>
@@ -91,15 +85,9 @@
     <t xml:space="preserve">(Präsenz) Wissenschaftliches Lesen II: Literaturreviews und Recherche </t>
   </si>
   <si>
-    <t xml:space="preserve">(Präsenz) Quantitative Methoden II – Logik der quantitativen Methoden </t>
-  </si>
-  <si>
     <t>(Online) Sprechstunde für Hausarbeiten 1</t>
   </si>
   <si>
-    <t xml:space="preserve">(Asynchron) Quantitative Methoden III – Daten reinigen und visualisieren </t>
-  </si>
-  <si>
     <t>(Präsenz) Quantitative Methoden V – Anwendung 2</t>
   </si>
   <si>
@@ -110,6 +98,18 @@
   </si>
   <si>
     <t>(Online) Sprechstunde für Hausarbeiten 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Bibliothek + Asynchron) Wahlen und Wähler in Deutschland und der Welt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Asynchron) Quantitative Methoden II – Daten reinigen und visualisieren </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Präsenz) Quantitative Methoden III – Logik der quantitativen Methoden </t>
+  </si>
+  <si>
+    <t>(Asynchron) Quantitative Methoden IV – Anwendung 1</t>
   </si>
 </sst>
 </file>
@@ -119,7 +119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m\.yy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,13 +146,27 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -167,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -184,18 +198,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -537,7 +548,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C21" sqref="C21:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +589,7 @@
         <v>45215</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="5" t="str">
         <f>_xlfn.CONCAT(A4,": ",C4)</f>
@@ -595,7 +606,7 @@
         <v>45222</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="str">
         <f t="shared" ref="D5:D19" si="0">_xlfn.CONCAT(A5,": ",C5)</f>
@@ -612,7 +623,7 @@
         <v>45229</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="5" t="str">
         <f t="shared" si="0"/>
@@ -629,7 +640,7 @@
         <v>45236</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="5" t="str">
         <f t="shared" ref="D7:D11" si="2">_xlfn.CONCAT(A7,": ",C7)</f>
@@ -645,12 +656,12 @@
         <f t="shared" ref="B8:B19" si="3">B7+7</f>
         <v>45243</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>10</v>
+      <c r="C8" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="D8" s="5" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">5: (Asynchron+Online) Wahlen und Wähler in Deutschland und der Welt </v>
+        <v xml:space="preserve">5: (Bibliothek + Asynchron) Wahlen und Wähler in Deutschland und der Welt </v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -663,11 +674,11 @@
         <v>45250</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>6: (Präsenz) Wer wählt populistische Parteien? + Wissenschaftliches Lesen I</v>
+        <f>_xlfn.CONCAT(A9,": ",C9)</f>
+        <v xml:space="preserve">6: (Asynchron) Quantitative Methoden I - Einführung in R </v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -680,11 +691,11 @@
         <v>45257</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">7: (Asynchron) Quantitative Methoden I - Einführung in R </v>
+        <f>_xlfn.CONCAT(A10,": ",C10)</f>
+        <v>7: (Präsenz) Wer wählt populistische Parteien? + Wissenschaftliches Lesen I</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -697,11 +708,11 @@
         <v>45264</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D11" s="5" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">8: (Präsenz) Wissenschaftliches Lesen II: Literaturreviews und Recherche </v>
+        <v xml:space="preserve">8: (Asynchron) Quantitative Methoden II – Daten reinigen und visualisieren </v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -714,11 +725,11 @@
         <v>45271</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="str">
         <f>_xlfn.CONCAT(A12,": ",C12)</f>
-        <v>9: (Online) Sprechstunde für Hausarbeiten 1</v>
+        <v xml:space="preserve">9: (Präsenz) Wissenschaftliches Lesen II: Literaturreviews und Recherche </v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -731,11 +742,11 @@
         <v>45278</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D13" s="5" t="str">
         <f>_xlfn.CONCAT(A13,": ",C13)</f>
-        <v xml:space="preserve">10: (Asynchron) Quantitative Methoden III – Daten reinigen und visualisieren </v>
+        <v>10: (Online) Sprechstunde für Hausarbeiten 1</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -746,12 +757,12 @@
       <c r="B14" s="6">
         <v>45299</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>20</v>
+      <c r="C14" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D14" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>11: (Online) Sprechstunde für Hausarbeiten 2</v>
+        <f>_xlfn.CONCAT(A14,": ",C14)</f>
+        <v xml:space="preserve">11: (Präsenz) Quantitative Methoden III – Logik der quantitativen Methoden </v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -764,11 +775,11 @@
         <v>45306</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D15" s="5" t="str">
         <f>_xlfn.CONCAT(A15,": ",C15)</f>
-        <v xml:space="preserve">12: (Präsenz) Quantitative Methoden II – Logik der quantitativen Methoden </v>
+        <v>12: (Asynchron) Quantitative Methoden IV – Anwendung 1</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -781,11 +792,11 @@
         <v>45313</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D16" s="5" t="str">
         <f>_xlfn.CONCAT(A16,": ",C16)</f>
-        <v>13: Quantitative Methoden IV – Anwendung 1</v>
+        <v>13: (Präsenz) Quantitative Methoden V – Anwendung 2</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -798,11 +809,11 @@
         <v>45320</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D17" s="5" t="str">
         <f>_xlfn.CONCAT(A17,": ",C17)</f>
-        <v>14: (Präsenz) Quantitative Methoden V – Anwendung 2</v>
+        <v xml:space="preserve">14: (Präsenz) Qualitative Methoden </v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -815,11 +826,11 @@
         <v>45327</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D18" s="5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">15: (Präsenz) Qualitative Methoden </v>
+        <v>15: (Online) Sprechstunde für Hausarbeiten 2</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -832,7 +843,7 @@
         <v>45334</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D19" s="5" t="str">
         <f t="shared" si="0"/>
@@ -859,18 +870,34 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="11"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C28" s="8"/>
+    </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C30" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C25 C4:C19">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>ISNUMBER(SEARCH("(Präsenz)", C4:C19))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>ISNUMBER(SEARCH("(Präsenz)", C13:C28))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>ISNUMBER(SEARCH("(Präsenz)", C28:C43))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>ISNUMBER(SEARCH("(Präsenz)", C15:C29))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>